<commit_message>
fix description bug add AbstractTaiwuPower
</commit_message>
<xml_diff>
--- a/src/main/resources/data/太吾尖塔.xlsx
+++ b/src/main/resources/data/太吾尖塔.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="149">
   <si>
     <t>ID</t>
   </si>
@@ -143,28 +143,28 @@
     <t>SKILL</t>
   </si>
   <si>
+    <t>SELF</t>
+  </si>
+  <si>
+    <t>移*1</t>
+  </si>
+  <si>
+    <t>获得 B 点格挡。</t>
+  </si>
+  <si>
+    <t>大拙手</t>
+  </si>
+  <si>
+    <t>DaZhuoShou</t>
+  </si>
+  <si>
     <t>RARE</t>
   </si>
   <si>
-    <t>SELF</t>
-  </si>
-  <si>
-    <t>移*1</t>
-  </si>
-  <si>
-    <t>获得 B 点格挡。</t>
-  </si>
-  <si>
-    <t>大拙手</t>
-  </si>
-  <si>
-    <t>DaZhuoShou</t>
-  </si>
-  <si>
     <t>崩*5</t>
   </si>
   <si>
-    <t>造成 D1 + D2 + D3 + D4 点伤害，若完全被对方格挡，立刻再次释放大拙手攻击敌人，且威力提升50%，直到造成伤害为止。</t>
+    <t>造成 S1 + S2 + S3 + S4 点伤害，若完全被对方格挡，立刻再次释放大拙手攻击敌人，且威力提升50%，直到造成伤害为止。</t>
   </si>
   <si>
     <t>0|0|10|10</t>
@@ -302,7 +302,7 @@
     <t>拿*2</t>
   </si>
   <si>
-    <t>造成 D1 + D2 + D3 + D4 点伤害，获得 M 层卸力。</t>
+    <t>造成 S1 + S2 + S3 + S4 点伤害，获得 M 层卸力。</t>
   </si>
   <si>
     <t>3|5|2|10</t>
@@ -323,13 +323,10 @@
     <t>XuanGongShenQuan</t>
   </si>
   <si>
-    <t>拿,1</t>
-  </si>
-  <si>
     <t>拿*3</t>
   </si>
   <si>
-    <t>造成 D1 + D2 + D3 + D4 点伤害，最后一段伤害额外附加当前卸力层数 M 倍的伤害。</t>
+    <t>造成 S1 + S2 + S3 + S4 点伤害，最后一段伤害额外附加当前卸力层数 M 倍的伤害。</t>
   </si>
   <si>
     <t>三华聚顶</t>
@@ -359,7 +356,7 @@
     <t>拿*2&amp;点*2&amp;崩*2</t>
   </si>
   <si>
-    <t>对所有敌人造成 D1 + D2 + D3 + D4 点伤害。</t>
+    <t>对所有敌人造成 S1 + S2 + S3 + S4 点伤害。</t>
   </si>
   <si>
     <t>2|8|0|10</t>
@@ -410,7 +407,7 @@
     <t>点*2</t>
   </si>
   <si>
-    <t>造成 D1 + D2 + D3 + D4 点伤害，附加 M 层虚弱。</t>
+    <t>造成 S1 + S2 + S3 + S4 点伤害，附加 M 层虚弱。</t>
   </si>
   <si>
     <t>4|2|4|10</t>
@@ -422,7 +419,7 @@
     <t>SuoHouYinShou</t>
   </si>
   <si>
-    <t>造成 D1 + D2 + D3 + D4 点伤害。本回合每打出一张牌，对目标造成 M 点伤害。</t>
+    <t>造成 S1 + S2 + S3 + S4 点伤害。本回合每打出一张牌，对目标造成 M 点伤害。</t>
   </si>
   <si>
     <t>4|3|3|10</t>
@@ -434,7 +431,7 @@
     <t>SanZhiDuoYinZhua</t>
   </si>
   <si>
-    <t>造成 D1 + D2 + D3 + D4 点伤害，附加 M 层易伤并击晕一回合。消耗。</t>
+    <t>造成 S1 + S2 + S3 + S4 点伤害，附加 M 层易伤并击晕一回合。消耗。</t>
   </si>
   <si>
     <t>移魂大法</t>
@@ -1825,18 +1822,18 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:xvml="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:pvml="urn:schemas-microsoft-com:office:powerpoint" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas">
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:xvml="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:pvml="urn:schemas-microsoft-com:office:powerpoint" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360000" cy="381000"/>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631190020560-dd9d213092818080" descr="attachment-1631190020560-dd9d213092818080"/>
+        <xdr:cNvPr id="1" name="attachment-1631190035646-e14fc2ef71609b4b" descr="attachment-1631190035646-e14fc2ef71609b4b"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1862,13 +1859,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360000" cy="381000"/>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631192947879-92f2c94add253548" descr="attachment-1631192947879-92f2c94add253548"/>
+        <xdr:cNvPr id="1" name="attachment-1631190048398-416111b891f295e2" descr="attachment-1631190048398-416111b891f295e2"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1894,13 +1891,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="360000" cy="381000"/>
+    <xdr:ext cx="360000" cy="533400"/>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631192990352-3f414e449418e62f" descr="attachment-1631192990352-3f414e449418e62f"/>
+        <xdr:cNvPr id="1" name="attachment-1631169939534-e5b91541e745fb8d" descr="attachment-1631169939534-e5b91541e745fb8d"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1912,7 +1909,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="0">
-          <a:ext cx="360000" cy="381000"/>
+          <a:ext cx="360000" cy="533400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1926,13 +1923,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360000" cy="381000"/>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631192963683-d029256278ba32e6" descr="attachment-1631192963683-d029256278ba32e6"/>
+        <xdr:cNvPr id="1" name="attachment-1631190064925-900f88ae6b4f5f8d" descr="attachment-1631190064925-900f88ae6b4f5f8d"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1990,17 +1987,49 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360000" cy="381000"/>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631190064925-900f88ae6b4f5f8d" descr="attachment-1631190064925-900f88ae6b4f5f8d"/>
+        <xdr:cNvPr id="1" name="attachment-1631190020560-dd9d213092818080" descr="attachment-1631190020560-dd9d213092818080"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip cstate="print" r:embed="rId6" r:link=""/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect l="0" t="0" r="0" b="0"/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0">
+          <a:ext cx="360000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360000" cy="381000"/>
+    <xdr:pic macro="">
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="attachment-1631192947879-92f2c94add253548" descr="attachment-1631192947879-92f2c94add253548"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId7" r:link=""/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect l="0" t="0" r="0" b="0"/>
@@ -2032,38 +2061,6 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId7" r:link=""/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect l="0" t="0" r="0" b="0"/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="0">
-          <a:ext cx="360000" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="360000" cy="381000"/>
-    <xdr:pic macro="">
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631190035646-e14fc2ef71609b4b" descr="attachment-1631190035646-e14fc2ef71609b4b"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
         <a:blip cstate="print" r:embed="rId8" r:link=""/>
         <a:srcRect/>
         <a:stretch>
@@ -2086,13 +2083,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="360000" cy="533400"/>
+    <xdr:ext cx="360000" cy="381000"/>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631169939534-e5b91541e745fb8d" descr="attachment-1631169939534-e5b91541e745fb8d"/>
+        <xdr:cNvPr id="1" name="attachment-1631192963683-d029256278ba32e6" descr="attachment-1631192963683-d029256278ba32e6"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2104,7 +2101,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="0">
-          <a:ext cx="360000" cy="533400"/>
+          <a:ext cx="360000" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2118,13 +2115,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360000" cy="381000"/>
     <xdr:pic macro="">
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="attachment-1631190048398-416111b891f295e2" descr="attachment-1631190048398-416111b891f295e2"/>
+        <xdr:cNvPr id="1" name="attachment-1631192990352-3f414e449418e62f" descr="attachment-1631192990352-3f414e449418e62f"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2622,10 +2619,10 @@
         <v>42</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -2642,10 +2639,10 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="V6" s="2"/>
       <c r="W6" s="1"/>
@@ -2671,10 +2668,10 @@
     </row>
     <row r="7" ht="56.0" customHeight="true">
       <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="n">
@@ -2688,7 +2685,7 @@
         <v>29</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>31</v>
@@ -2771,7 +2768,7 @@
         <v>57</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -2835,7 +2832,7 @@
         <v>57</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2896,10 +2893,10 @@
         <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -2961,7 +2958,7 @@
         <v>57</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -3025,7 +3022,7 @@
         <v>57</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -3293,7 +3290,7 @@
         <v>73</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -3357,7 +3354,7 @@
         <v>73</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -3422,10 +3419,10 @@
         <v>56</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -3491,7 +3488,7 @@
         <v>57</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -3714,7 +3711,7 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="1" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>33</v>
@@ -3723,10 +3720,10 @@
         <v>52</v>
       </c>
       <c r="W22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X22" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="Y22" s="1" t="s">
         <v>97</v>
@@ -3751,10 +3748,10 @@
     </row>
     <row r="23" ht="40.0" customHeight="true">
       <c r="A23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="n">
@@ -3770,10 +3767,10 @@
         <v>42</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -3786,10 +3783,10 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="U23" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
@@ -3815,10 +3812,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="n">
@@ -3832,10 +3829,10 @@
         <v>29</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J24" s="2" t="n">
         <v>30.0</v>
@@ -3857,19 +3854,19 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V24" s="2" t="s">
         <v>52</v>
       </c>
       <c r="W24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="X24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="X24" s="1" t="s">
+      <c r="Y24" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="Y24" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
@@ -3891,10 +3888,10 @@
     </row>
     <row r="25" ht="30.0" customHeight="true">
       <c r="A25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="n">
@@ -3911,7 +3908,7 @@
         <v>57</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -3929,7 +3926,7 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
@@ -3955,10 +3952,10 @@
     </row>
     <row r="26" ht="40.0" customHeight="true">
       <c r="A26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="n">
@@ -3975,7 +3972,7 @@
         <v>57</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -3997,7 +3994,7 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
@@ -4023,10 +4020,10 @@
     </row>
     <row r="27" ht="30.0" customHeight="true">
       <c r="A27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="n">
@@ -4043,7 +4040,7 @@
         <v>73</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -4065,7 +4062,7 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
@@ -4091,10 +4088,10 @@
     </row>
     <row r="28" ht="40.0" customHeight="true">
       <c r="A28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="n">
@@ -4137,7 +4134,7 @@
       </c>
       <c r="T28" s="2"/>
       <c r="U28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
@@ -4163,10 +4160,10 @@
     </row>
     <row r="29" ht="30.0" customHeight="true">
       <c r="A29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="n">
@@ -4211,13 +4208,13 @@
       </c>
       <c r="V29" s="2"/>
       <c r="W29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="X29" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="X29" s="1" t="s">
+      <c r="Y29" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="Y29" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
@@ -4239,10 +4236,10 @@
     </row>
     <row r="30" ht="40.0" customHeight="true">
       <c r="A30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="n">
@@ -4287,13 +4284,13 @@
       </c>
       <c r="V30" s="2"/>
       <c r="W30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y30" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="Y30" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
@@ -4315,10 +4312,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="n">
@@ -4363,13 +4360,13 @@
       </c>
       <c r="V31" s="2"/>
       <c r="W31" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
@@ -4391,10 +4388,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="n">
@@ -4408,10 +4405,10 @@
         <v>42</v>
       </c>
       <c r="H32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -4429,7 +4426,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
@@ -4455,10 +4452,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="n">
@@ -4472,10 +4469,10 @@
         <v>56</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -4497,7 +4494,7 @@
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
@@ -4523,10 +4520,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="n">
@@ -4545,7 +4542,7 @@
         <v>57</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -4563,7 +4560,7 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>

</xml_diff>